<commit_message>
Uploaded 18-Jan-2019 05:12:50 {/src/main/resources/com/myspace/shipping_quote/determine price by distance.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/shipping_quote/determine price by distance.xlsx
+++ b/src/main/resources/com/myspace/shipping_quote/determine price by distance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Medium trip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium large trip</t>
   </si>
   <si>
     <t xml:space="preserve">Large trip</t>
@@ -94,6 +97,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -115,12 +119,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -128,6 +134,7 @@
       <color rgb="FFFFFFD7"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -187,11 +194,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,16 +283,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
@@ -378,7 +384,7 @@
         <v>150</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,10 +409,24 @@
         <v>300</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>600</v>
+        <v>450</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>450</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>